<commit_message>
In blue are the ones I implemented.
</commit_message>
<xml_diff>
--- a/Knowledge Base.xlsx
+++ b/Knowledge Base.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abrah\Desktop\CS3520\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\impet\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3690C15E-E751-419D-814A-C7A9E78DE5B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="240"/>
+    <workbookView xWindow="17925" yWindow="3240" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -110,7 +111,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -148,7 +149,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,6 +175,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -207,7 +214,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -233,6 +240,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -514,11 +525,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,131 +982,131 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" t="s">
-        <v>13</v>
-      </c>
-      <c r="J16" t="s">
-        <v>13</v>
-      </c>
-      <c r="K16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C16" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="13" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H17" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" t="s">
-        <v>15</v>
-      </c>
-      <c r="K17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="C17" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" t="s">
-        <v>14</v>
-      </c>
-      <c r="J18" t="s">
-        <v>13</v>
-      </c>
-      <c r="K18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" t="s">
-        <v>15</v>
-      </c>
-      <c r="J19" t="s">
-        <v>15</v>
-      </c>
-      <c r="K19" t="s">
+      <c r="C19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" s="13" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>